<commit_message>
added assets and type of plot
</commit_message>
<xml_diff>
--- a/data/pollution_data.xlsx
+++ b/data/pollution_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51ae962a39f43cd0/Pulpit/Marcysia/github/visualisation_geographic_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{32D97925-EDF2-4026-9521-DCAA707596EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{784058CB-2E03-4EA0-B3A9-D589E3654281}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{32D97925-EDF2-4026-9521-DCAA707596EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75A1B72-4763-4CE8-B0DA-8B807BE9A658}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{464988A6-2CE5-4FD1-850F-A329DDD75F44}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="24">
   <si>
     <t>kujawsko-pomorskie</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>warminsko-mazurskie</t>
+  </si>
+  <si>
+    <t>area</t>
   </si>
 </sst>
 </file>
@@ -698,30 +701,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="22" fillId="0" borderId="11" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="11" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="11" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="11" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="22" fillId="0" borderId="11" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -922,6 +907,10 @@
 </file>
 
 <file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1222,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7818F3A-23A1-49D0-83E8-3B6A860DDD22}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="A1:G17"/>
+      <selection activeCell="B1" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1233,394 +1222,445 @@
     <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
+        <v>19947</v>
+      </c>
+      <c r="C2" s="2">
         <v>18053.82051281862</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>62.29219059092754</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>3.0370269544038444</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>26.119572311496484</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>32.545935449581393</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>133.64349072015318</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
+        <v>17972</v>
+      </c>
+      <c r="C3" s="2">
         <v>14428.389148573677</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>70.175726900002573</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>6.281156009926093</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>35.620070123474228</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>45.696579050983857</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>165.4849544552338</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
+        <v>25122</v>
+      </c>
+      <c r="C4" s="2">
         <v>11941.273729358196</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>127.01853433796794</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>6.0475324976840259</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>24.647847397626251</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>32.570207674107102</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>129.37753905956953</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
+        <v>13988</v>
+      </c>
+      <c r="C5" s="2">
         <v>4394.4002262132408</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>48.972046782867857</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>1.5968037448055219</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>4.3647295278585858</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>10.649865702808492</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>46.620111171837642</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
+        <v>18219</v>
+      </c>
+      <c r="C6" s="2">
         <v>44628.606294883604</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>107.7451179087455</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>5.3236955142290947</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>57.244957337036716</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>63.866215804387259</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>191.37368495330725</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
+        <v>15183</v>
+      </c>
+      <c r="C7" s="2">
         <v>17126.873627445228</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>69.491193194909528</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>2.3087305137438485</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>28.241316156380663</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>37.661365263433133</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>174.46034084347582</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
+        <v>35558</v>
+      </c>
+      <c r="C8" s="2">
         <v>58606.328830972612</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>175.72466591051042</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>9.9498833825560773</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>61.578370288798702</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>97.250798261788319</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>246.05624240312667</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
+        <v>9412</v>
+      </c>
+      <c r="C9" s="2">
         <v>18684.700246930697</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>27.495768589952029</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>2.6281131390360422</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>13.949306499465544</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>21.256981241606837</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>60.711634925717831</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
+        <v>17846</v>
+      </c>
+      <c r="C10" s="2">
         <v>7633.7585877836527</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>37.6737821807016</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>1.5178409393179679</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>17.330079860980856</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>22.386329004741899</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>178.86112761161121</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
+        <v>20187</v>
+      </c>
+      <c r="C11" s="2">
         <v>3704.2814462801784</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>105.33129286605737</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>7.1751796387407571</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>7.8711125354572715</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>17.962153638495163</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>56.56560559220879</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
+        <v>18310</v>
+      </c>
+      <c r="C12" s="2">
         <v>12342.014001447867</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>63.523041265664418</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>3.9094875297270981</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>27.080986029990164</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>34.023540401548182</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>145.61588674994019</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
+        <v>12333</v>
+      </c>
+      <c r="C13" s="2">
         <v>42904.495170288268</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>577.88090456230179</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>2.4930787119202962</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>43.646762943152602</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>50.506979837898264</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>214.45822647592777</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
+        <v>11711</v>
+      </c>
+      <c r="C14" s="2">
         <v>13903.503526821161</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>28.973897396069653</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>1.8624633836003193</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>20.959282302117813</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>23.731190137092945</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>67.672660320798713</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
+        <v>24173</v>
+      </c>
+      <c r="C15" s="2">
         <v>5148.4136531310787</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>63.115755000661039</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>5.4811273051909133</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>12.118157762941715</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>19.633184520894467</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>76.422446252651881</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
+        <v>29826</v>
+      </c>
+      <c r="C16" s="2">
         <v>19690.86654134755</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>160.45237555808635</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>11.327513983744511</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>28.463576691477115</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>52.348091268444755</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>185.15658801042389</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
+        <v>22892</v>
+      </c>
+      <c r="C17" s="2">
         <v>10331.356342396966</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>48.365900130330132</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>5.7008046422090732</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>22.647497380060965</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>31.815345134135661</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>126.33843894425631</v>
       </c>
     </row>
@@ -1631,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8598B8FC-B048-4239-964A-724689BBF094}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G17"/>
+      <selection activeCell="B1" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1642,394 +1682,445 @@
     <col min="1" max="1" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
+        <v>19947</v>
+      </c>
+      <c r="C2" s="2">
         <v>19663.332794687922</v>
       </c>
-      <c r="C2" s="4">
+      <c r="D2" s="2">
         <v>65.374499708505496</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="2">
         <v>2.9628361664411664</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="2">
         <v>23.774235956611296</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="2">
         <v>41.880016736269198</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="2">
         <v>129.12861739325157</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
+        <v>17972</v>
+      </c>
+      <c r="C3" s="2">
         <v>12495.309085256238</v>
       </c>
-      <c r="C3" s="4">
+      <c r="D3" s="2">
         <v>72.130393676834728</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="2">
         <v>5.9326092433782076</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="2">
         <v>36.379858320402811</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="2">
         <v>43.809323289456174</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="2">
         <v>151.59800216712677</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
+        <v>25122</v>
+      </c>
+      <c r="C4" s="2">
         <v>13018.50963886369</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="2">
         <v>124.84804793862905</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="2">
         <v>6.4449118295486443</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="2">
         <v>23.204103220511801</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="2">
         <v>42.924010799607856</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="2">
         <v>128.46492161414466</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
+        <v>13988</v>
+      </c>
+      <c r="C5" s="2">
         <v>5300.6212539601565</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="2">
         <v>51.626177686111347</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="2">
         <v>1.6178033219489307</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="2">
         <v>3.9103116721625022</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="2">
         <v>17.145860310578946</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="2">
         <v>48.282301498348517</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
+        <v>18219</v>
+      </c>
+      <c r="C6" s="2">
         <v>44649.70643640557</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="2">
         <v>112.48041477508079</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="2">
         <v>5.0039990786152471</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="2">
         <v>51.00131371924536</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="2">
         <v>67.116127385661855</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="2">
         <v>169.64045768281625</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
+        <v>15183</v>
+      </c>
+      <c r="C7" s="2">
         <v>22504.393298967731</v>
       </c>
-      <c r="C7" s="4">
+      <c r="D7" s="2">
         <v>71.760244348374925</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="2">
         <v>2.7090642799958182</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="2">
         <v>42.694623256044366</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="2">
         <v>45.414651363193009</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="2">
         <v>165.20564830335471</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
+        <v>35558</v>
+      </c>
+      <c r="C8" s="2">
         <v>59624.590670301601</v>
       </c>
-      <c r="C8" s="4">
+      <c r="D8" s="2">
         <v>187.16584957707465</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="2">
         <v>9.3649752625338092</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="2">
         <v>71.39877642045299</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="2">
         <v>106.13242403456194</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="2">
         <v>240.72788125526688</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
+        <v>9412</v>
+      </c>
+      <c r="C9" s="2">
         <v>19595.052241510992</v>
       </c>
-      <c r="C9" s="4">
+      <c r="D9" s="2">
         <v>28.901062914396174</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="2">
         <v>2.5690929595851881</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="2">
         <v>13.990530364688231</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="2">
         <v>27.299315280781808</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="2">
         <v>64.323990900352953</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
+        <v>17846</v>
+      </c>
+      <c r="C10" s="2">
         <v>8238.0278221656172</v>
       </c>
-      <c r="C10" s="4">
+      <c r="D10" s="2">
         <v>39.735124483436991</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="2">
         <v>1.5011751000839901</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="2">
         <v>14.185831734253451</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="2">
         <v>26.803761381140159</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="2">
         <v>189.60326577433452</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
+        <v>20187</v>
+      </c>
+      <c r="C11" s="2">
         <v>4527.5579701004835</v>
       </c>
-      <c r="C11" s="4">
+      <c r="D11" s="2">
         <v>103.70187906983413</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="2">
         <v>6.83075490479085</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="2">
         <v>7.628055043669832</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="2">
         <v>22.476076500875298</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="2">
         <v>53.704201336316601</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
+        <v>18310</v>
+      </c>
+      <c r="C12" s="2">
         <v>10963.171654863636</v>
       </c>
-      <c r="C12" s="4">
+      <c r="D12" s="2">
         <v>63.983363778721554</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="2">
         <v>3.7624356397524887</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="2">
         <v>19.612156264105725</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="2">
         <v>33.209331309051962</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="2">
         <v>133.0162826956151</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
+        <v>12333</v>
+      </c>
+      <c r="C13" s="2">
         <v>44308.146775206013</v>
       </c>
-      <c r="C13" s="4">
+      <c r="D13" s="2">
         <v>587.91825227068796</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="2">
         <v>2.431901321898001</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="2">
         <v>36.897660012446721</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="2">
         <v>58.180839853886461</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="2">
         <v>192.35382814136943</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
+        <v>11711</v>
+      </c>
+      <c r="C14" s="2">
         <v>16592.006196148086</v>
       </c>
-      <c r="C14" s="4">
+      <c r="D14" s="2">
         <v>29.877763848036519</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="2">
         <v>1.8043810938249105</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="2">
         <v>21.10424922877532</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="2">
         <v>30.096280604253433</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="2">
         <v>69.957254449589627</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
+        <v>24173</v>
+      </c>
+      <c r="C15" s="2">
         <v>5160.6721386193758</v>
       </c>
-      <c r="C15" s="4">
+      <c r="D15" s="2">
         <v>61.490734313199432</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="2">
         <v>5.0329916437987299</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="2">
         <v>11.380676411263954</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="2">
         <v>20.597279715321072</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="2">
         <v>75.112495374663297</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
+        <v>29826</v>
+      </c>
+      <c r="C16" s="2">
         <v>22806.024296914991</v>
       </c>
-      <c r="C16" s="4">
+      <c r="D16" s="2">
         <v>160.41762698247223</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="2">
         <v>10.567061532204358</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="2">
         <v>26.018700746841748</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="2">
         <v>65.974669071470814</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="2">
         <v>185.38781330574918</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
+        <v>22892</v>
+      </c>
+      <c r="C17" s="2">
         <v>10073.852333251958</v>
       </c>
-      <c r="C17" s="4">
+      <c r="D17" s="2">
         <v>49.640544439624193</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E17" s="2">
         <v>5.6291246333743938</v>
       </c>
-      <c r="E17" s="4">
+      <c r="F17" s="2">
         <v>23.815293530342711</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="2">
         <v>32.461079441906705</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="2">
         <v>115.44561401446936</v>
       </c>
     </row>
@@ -2040,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4806FBA-1A1C-40A4-9BED-5BA200EFD858}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="A1:G17"/>
+      <selection activeCell="B1" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2051,394 +2142,445 @@
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2">
+        <v>19947</v>
+      </c>
+      <c r="C2" s="2">
         <v>21767.767246560019</v>
       </c>
-      <c r="C2" s="6">
+      <c r="D2" s="2">
         <v>70.011910745739826</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="2">
         <v>3.1197319860031292</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="2">
         <v>32.422160932769714</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="2">
         <v>50.640634706602583</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="2">
         <v>149.01959561039246</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3">
+        <v>17972</v>
+      </c>
+      <c r="C3" s="2">
         <v>12794.097168476022</v>
       </c>
-      <c r="C3" s="6">
+      <c r="D3" s="2">
         <v>76.164586248437928</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="2">
         <v>6.1454541487813543</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="2">
         <v>39.812513485555144</v>
       </c>
-      <c r="F3" s="6">
+      <c r="G3" s="2">
         <v>49.830561663124236</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="2">
         <v>154.12010727836878</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4">
+        <v>25122</v>
+      </c>
+      <c r="C4" s="2">
         <v>13230.258489990845</v>
       </c>
-      <c r="C4" s="6">
+      <c r="D4" s="2">
         <v>132.33020285138576</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="2">
         <v>6.602328796918405</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="2">
         <v>26.093290696594931</v>
       </c>
-      <c r="F4" s="6">
+      <c r="G4" s="2">
         <v>46.678426287258958</v>
       </c>
-      <c r="G4" s="6">
+      <c r="H4" s="2">
         <v>139.64958254621368</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
+        <v>13988</v>
+      </c>
+      <c r="C5" s="2">
         <v>5389.5430053007622</v>
       </c>
-      <c r="C5" s="6">
+      <c r="D5" s="2">
         <v>53.84949106021471</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="2">
         <v>1.6241897217725842</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="2">
         <v>4.4203762677632463</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="2">
         <v>18.565401629026184</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="2">
         <v>51.353439429577968</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
+        <v>18219</v>
+      </c>
+      <c r="C6" s="2">
         <v>51116.149365806275</v>
       </c>
-      <c r="C6" s="6">
+      <c r="D6" s="2">
         <v>122.86722534299147</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="2">
         <v>4.8815114716933827</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="2">
         <v>72.267256117479135</v>
       </c>
-      <c r="F6" s="6">
+      <c r="G6" s="2">
         <v>74.675398565418845</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="2">
         <v>180.86112169103038</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
+        <v>15183</v>
+      </c>
+      <c r="C7" s="2">
         <v>24711.589327360409</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D7" s="2">
         <v>76.673165226841022</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="2">
         <v>2.6859830927951505</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="2">
         <v>50.269481032948114</v>
       </c>
-      <c r="F7" s="6">
+      <c r="G7" s="2">
         <v>49.905227588123978</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="2">
         <v>191.76608208093342</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
+        <v>35558</v>
+      </c>
+      <c r="C8" s="2">
         <v>58367.095743931204</v>
       </c>
-      <c r="C8" s="6">
+      <c r="D8" s="2">
         <v>188.14919583334952</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="2">
         <v>9.6665085990387958</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="2">
         <v>73.245317620190391</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="2">
         <v>109.83270433338389</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="2">
         <v>267.40492637934102</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
+        <v>9412</v>
+      </c>
+      <c r="C9" s="2">
         <v>17693.755469468906</v>
       </c>
-      <c r="C9" s="6">
+      <c r="D9" s="2">
         <v>30.847834941488969</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="2">
         <v>2.6105668958509263</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="2">
         <v>14.890063018158866</v>
       </c>
-      <c r="F9" s="6">
+      <c r="G9" s="2">
         <v>30.524280669901582</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="2">
         <v>64.426949710375126</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
+        <v>17846</v>
+      </c>
+      <c r="C10" s="2">
         <v>8227.2685467201627</v>
       </c>
-      <c r="C10" s="6">
+      <c r="D10" s="2">
         <v>42.573559803021247</v>
       </c>
-      <c r="D10" s="6">
+      <c r="E10" s="2">
         <v>1.4975660301639566</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F10" s="2">
         <v>15.764720249223222</v>
       </c>
-      <c r="F10" s="6">
+      <c r="G10" s="2">
         <v>27.019400905814202</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="2">
         <v>228.71068407201852</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11">
+        <v>20187</v>
+      </c>
+      <c r="C11" s="2">
         <v>4691.1474099279112</v>
       </c>
-      <c r="C11" s="6">
+      <c r="D11" s="2">
         <v>110.77202106390831</v>
       </c>
-      <c r="D11" s="6">
+      <c r="E11" s="2">
         <v>6.6339440153064855</v>
       </c>
-      <c r="E11" s="6">
+      <c r="F11" s="2">
         <v>9.2443695101175436</v>
       </c>
-      <c r="F11" s="6">
+      <c r="G11" s="2">
         <v>22.611258030554687</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="2">
         <v>62.266036136612527</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12">
+        <v>18310</v>
+      </c>
+      <c r="C12" s="2">
         <v>11340.754280772973</v>
       </c>
-      <c r="C12" s="6">
+      <c r="D12" s="2">
         <v>68.673679439878043</v>
       </c>
-      <c r="D12" s="6">
+      <c r="E12" s="2">
         <v>3.5723933737759692</v>
       </c>
-      <c r="E12" s="6">
+      <c r="F12" s="2">
         <v>23.691722795525575</v>
       </c>
-      <c r="F12" s="6">
+      <c r="G12" s="2">
         <v>36.987999577701224</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="2">
         <v>148.04351473072992</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13">
+        <v>12333</v>
+      </c>
+      <c r="C13" s="2">
         <v>49612.105606190351</v>
       </c>
-      <c r="C13" s="6">
+      <c r="D13" s="2">
         <v>658.79070877161951</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="2">
         <v>2.4698753009621988</v>
       </c>
-      <c r="E13" s="6">
+      <c r="F13" s="2">
         <v>47.306247835083759</v>
       </c>
-      <c r="F13" s="6">
+      <c r="G13" s="2">
         <v>70.202124269719619</v>
       </c>
-      <c r="G13" s="6">
+      <c r="H13" s="2">
         <v>231.07457987768561</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14">
+        <v>11711</v>
+      </c>
+      <c r="C14" s="2">
         <v>18321.543792457007</v>
       </c>
-      <c r="C14" s="6">
+      <c r="D14" s="2">
         <v>32.39660931893178</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="2">
         <v>1.8721276943788978</v>
       </c>
-      <c r="E14" s="6">
+      <c r="F14" s="2">
         <v>23.279685328975418</v>
       </c>
-      <c r="F14" s="6">
+      <c r="G14" s="2">
         <v>31.516192310314189</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="2">
         <v>76.967224629009962</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15">
+        <v>24173</v>
+      </c>
+      <c r="C15" s="2">
         <v>5371.4887097163346</v>
       </c>
-      <c r="C15" s="6">
+      <c r="D15" s="2">
         <v>66.591523108345982</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="2">
         <v>5.0497756784735524</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F15" s="2">
         <v>13.264207818357741</v>
       </c>
-      <c r="F15" s="6">
+      <c r="G15" s="2">
         <v>25.561524469976217</v>
       </c>
-      <c r="G15" s="6">
+      <c r="H15" s="2">
         <v>65.104217195648545</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16">
+        <v>29826</v>
+      </c>
+      <c r="C16" s="2">
         <v>23869.712657029104</v>
       </c>
-      <c r="C16" s="6">
+      <c r="D16" s="2">
         <v>167.80703039088462</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="2">
         <v>10.359677592548946</v>
       </c>
-      <c r="E16" s="6">
+      <c r="F16" s="2">
         <v>29.463728316092343</v>
       </c>
-      <c r="F16" s="6">
+      <c r="G16" s="2">
         <v>79.204379450199781</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H16" s="2">
         <v>203.37527889455527</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17">
+        <v>22892</v>
+      </c>
+      <c r="C17" s="2">
         <v>11201.465003301355</v>
       </c>
-      <c r="C17" s="6">
+      <c r="D17" s="2">
         <v>51.630103857815634</v>
       </c>
-      <c r="D17" s="6">
+      <c r="E17" s="2">
         <v>5.3895934513974417</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="2">
         <v>26.495785102641111</v>
       </c>
-      <c r="F17" s="6">
+      <c r="G17" s="2">
         <v>37.956299327199645</v>
       </c>
-      <c r="G17" s="6">
+      <c r="H17" s="2">
         <v>124.93115666911177</v>
       </c>
     </row>
@@ -2449,402 +2591,453 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2917CE5-29C7-4EC4-AAA8-6BF7913A090C}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G17"/>
+      <selection activeCell="B1" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" ht="24">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2">
+        <v>19947</v>
+      </c>
+      <c r="C2" s="3">
         <v>20875.41</v>
       </c>
-      <c r="C2" s="8">
+      <c r="D2" s="3">
         <v>73.040000000000006</v>
       </c>
-      <c r="D2" s="8">
+      <c r="E2" s="3">
         <v>3.14</v>
       </c>
-      <c r="E2" s="8">
+      <c r="F2" s="3">
         <v>32.47</v>
       </c>
-      <c r="F2" s="8">
+      <c r="G2" s="3">
         <v>47.64</v>
       </c>
-      <c r="G2" s="8">
+      <c r="H2" s="3">
         <v>137.1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:8" ht="24">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3">
+        <v>17972</v>
+      </c>
+      <c r="C3" s="3">
         <v>14277.39</v>
       </c>
-      <c r="C3" s="8">
+      <c r="D3" s="3">
         <v>73.47</v>
       </c>
-      <c r="D3" s="8">
+      <c r="E3" s="3">
         <v>6.05</v>
       </c>
-      <c r="E3" s="8">
+      <c r="F3" s="3">
         <v>50.95</v>
       </c>
-      <c r="F3" s="8">
+      <c r="G3" s="3">
         <v>58.09</v>
       </c>
-      <c r="G3" s="8">
+      <c r="H3" s="3">
         <v>171.76</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4">
+        <v>25122</v>
+      </c>
+      <c r="C4" s="3">
         <v>12669.1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="D4" s="3">
         <v>144.77000000000001</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="3">
         <v>6.35</v>
       </c>
-      <c r="E4" s="8">
+      <c r="F4" s="3">
         <v>28.91</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G4" s="3">
         <v>45.15</v>
       </c>
-      <c r="G4" s="8">
+      <c r="H4" s="3">
         <v>128.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
+        <v>13988</v>
+      </c>
+      <c r="C5" s="3">
         <v>6601.5</v>
       </c>
-      <c r="C5" s="8">
+      <c r="D5" s="3">
         <v>55.42</v>
       </c>
-      <c r="D5" s="8">
+      <c r="E5" s="3">
         <v>1.51</v>
       </c>
-      <c r="E5" s="8">
+      <c r="F5" s="3">
         <v>5.75</v>
       </c>
-      <c r="F5" s="8">
+      <c r="G5" s="3">
         <v>23.92</v>
       </c>
-      <c r="G5" s="8">
+      <c r="H5" s="3">
         <v>66.97</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
+        <v>18219</v>
+      </c>
+      <c r="C6" s="3">
         <v>49053.35</v>
       </c>
-      <c r="C6" s="8">
+      <c r="D6" s="3">
         <v>119.32</v>
       </c>
-      <c r="D6" s="8">
+      <c r="E6" s="3">
         <v>4.75</v>
       </c>
-      <c r="E6" s="8">
+      <c r="F6" s="3">
         <v>68.91</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G6" s="3">
         <v>73.14</v>
       </c>
-      <c r="G6" s="8">
+      <c r="H6" s="3">
         <v>157.88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="24">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:8" ht="24">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
+        <v>15183</v>
+      </c>
+      <c r="C7" s="3">
         <v>24883.21</v>
       </c>
-      <c r="C7" s="8">
+      <c r="D7" s="3">
         <v>76.59</v>
       </c>
-      <c r="D7" s="8">
+      <c r="E7" s="3">
         <v>2.77</v>
       </c>
-      <c r="E7" s="8">
+      <c r="F7" s="3">
         <v>68.930000000000007</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="3">
         <v>58.62</v>
       </c>
-      <c r="G7" s="8">
+      <c r="H7" s="3">
         <v>430.74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="24">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:8" ht="24">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
+        <v>35558</v>
+      </c>
+      <c r="C8" s="3">
         <v>49857.99</v>
       </c>
-      <c r="C8" s="8">
+      <c r="D8" s="3">
         <v>175.43</v>
       </c>
-      <c r="D8" s="8">
+      <c r="E8" s="3">
         <v>8.48</v>
       </c>
-      <c r="E8" s="8">
+      <c r="F8" s="3">
         <v>78.400000000000006</v>
       </c>
-      <c r="F8" s="8">
+      <c r="G8" s="3">
         <v>91.86</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="3">
         <v>355.84</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
+        <v>9412</v>
+      </c>
+      <c r="C9" s="3">
         <v>17669.990000000002</v>
       </c>
-      <c r="C9" s="8">
+      <c r="D9" s="3">
         <v>29.56</v>
       </c>
-      <c r="D9" s="8">
+      <c r="E9" s="3">
         <v>2.4900000000000002</v>
       </c>
-      <c r="E9" s="8">
+      <c r="F9" s="3">
         <v>17.649999999999999</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G9" s="3">
         <v>36.630000000000003</v>
       </c>
-      <c r="G9" s="8">
+      <c r="H9" s="3">
         <v>82.56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="24">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:8" ht="24">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
+        <v>17846</v>
+      </c>
+      <c r="C10" s="3">
         <v>8556.9699999999993</v>
       </c>
-      <c r="C10" s="8">
+      <c r="D10" s="3">
         <v>50.32</v>
       </c>
-      <c r="D10" s="8">
+      <c r="E10" s="3">
         <v>1.5</v>
       </c>
-      <c r="E10" s="8">
+      <c r="F10" s="3">
         <v>17.78</v>
       </c>
-      <c r="F10" s="8">
+      <c r="G10" s="3">
         <v>29.19</v>
       </c>
-      <c r="G10" s="8">
+      <c r="H10" s="3">
         <v>131.86000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
+        <v>20187</v>
+      </c>
+      <c r="C11" s="3">
         <v>5323.88</v>
       </c>
-      <c r="C11" s="8">
+      <c r="D11" s="3">
         <v>110.79</v>
       </c>
-      <c r="D11" s="8">
+      <c r="E11" s="3">
         <v>5.91</v>
       </c>
-      <c r="E11" s="8">
+      <c r="F11" s="3">
         <v>11.58</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="3">
         <v>26.11</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H11" s="3">
         <v>70.62</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
+        <v>18310</v>
+      </c>
+      <c r="C12" s="3">
         <v>13571.28</v>
       </c>
-      <c r="C12" s="8">
+      <c r="D12" s="3">
         <v>66.48</v>
       </c>
-      <c r="D12" s="8">
+      <c r="E12" s="3">
         <v>3.33</v>
       </c>
-      <c r="E12" s="8">
+      <c r="F12" s="3">
         <v>26.38</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G12" s="3">
         <v>45.79</v>
       </c>
-      <c r="G12" s="8">
+      <c r="H12" s="3">
         <v>116.46</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
+        <v>12333</v>
+      </c>
+      <c r="C13" s="3">
         <v>52791.73</v>
       </c>
-      <c r="C13" s="8">
+      <c r="D13" s="3">
         <v>662.53</v>
       </c>
-      <c r="D13" s="8">
+      <c r="E13" s="3">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E13" s="8">
+      <c r="F13" s="3">
         <v>62.45</v>
       </c>
-      <c r="F13" s="8">
+      <c r="G13" s="3">
         <v>82.99</v>
       </c>
-      <c r="G13" s="8">
+      <c r="H13" s="3">
         <v>241.36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="24">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:8" ht="24">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
+        <v>11711</v>
+      </c>
+      <c r="C14" s="3">
         <v>17261.62</v>
       </c>
-      <c r="C14" s="8">
+      <c r="D14" s="3">
         <v>32.090000000000003</v>
       </c>
-      <c r="D14" s="8">
+      <c r="E14" s="3">
         <v>1.88</v>
       </c>
-      <c r="E14" s="8">
+      <c r="F14" s="3">
         <v>22.92</v>
       </c>
-      <c r="F14" s="8">
+      <c r="G14" s="3">
         <v>37.909999999999997</v>
       </c>
-      <c r="G14" s="8">
+      <c r="H14" s="3">
         <v>87.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="24">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:8" ht="24">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
+        <v>24173</v>
+      </c>
+      <c r="C15" s="3">
         <v>6108.82</v>
       </c>
-      <c r="C15" s="8">
+      <c r="D15" s="3">
         <v>65.760000000000005</v>
       </c>
-      <c r="D15" s="8">
+      <c r="E15" s="3">
         <v>4.55</v>
       </c>
-      <c r="E15" s="8">
+      <c r="F15" s="3">
         <v>14.93</v>
       </c>
-      <c r="F15" s="8">
+      <c r="G15" s="3">
         <v>29.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="H15" s="3">
         <v>97.85</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="24">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:8" ht="24">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16">
+        <v>29826</v>
+      </c>
+      <c r="C16" s="3">
         <v>24640.12</v>
       </c>
-      <c r="C16" s="8">
+      <c r="D16" s="3">
         <v>188.84</v>
       </c>
-      <c r="D16" s="8">
+      <c r="E16" s="3">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E16" s="8">
+      <c r="F16" s="3">
         <v>47.15</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G16" s="3">
         <v>74.36</v>
       </c>
-      <c r="G16" s="8">
+      <c r="H16" s="3">
         <v>176.18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="24">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:8" ht="24">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17">
+        <v>22892</v>
+      </c>
+      <c r="C17" s="3">
         <v>12414.41</v>
       </c>
-      <c r="C17" s="8">
+      <c r="D17" s="3">
         <v>52.09</v>
       </c>
-      <c r="D17" s="8">
+      <c r="E17" s="3">
         <v>4.75</v>
       </c>
-      <c r="E17" s="8">
+      <c r="F17" s="3">
         <v>27.5</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="3">
         <v>42.93</v>
       </c>
-      <c r="G17" s="8">
+      <c r="H17" s="3">
         <v>90.54</v>
       </c>
     </row>
@@ -2855,10 +3048,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECAE9A7-1C24-431A-8CF3-7D2D22897543}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2866,394 +3059,445 @@
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2">
+        <v>19947</v>
+      </c>
+      <c r="C2" s="3">
         <v>20793.011135985849</v>
       </c>
-      <c r="C2" s="9">
+      <c r="D2" s="3">
         <v>65.337897819370312</v>
       </c>
-      <c r="D2" s="9">
+      <c r="E2" s="3">
         <v>2.8830272721955641</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F2" s="3">
         <v>50.499902802988359</v>
       </c>
-      <c r="F2" s="9">
+      <c r="G2" s="3">
         <v>52.283390256041535</v>
       </c>
-      <c r="G2" s="10">
+      <c r="H2" s="4">
         <v>172.22377097933506</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3">
+        <v>17972</v>
+      </c>
+      <c r="C3" s="3">
         <v>13909.223450114592</v>
       </c>
-      <c r="C3" s="9">
+      <c r="D3" s="3">
         <v>69.028254455958333</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E3" s="3">
         <v>5.564987088376351</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="3">
         <v>34.950791654384645</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="3">
         <v>51.66544009787853</v>
       </c>
-      <c r="G3" s="10">
+      <c r="H3" s="4">
         <v>145.93873708240068</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
+        <v>25122</v>
+      </c>
+      <c r="C4" s="3">
         <v>11981.390409204963</v>
       </c>
-      <c r="C4" s="9">
+      <c r="D4" s="3">
         <v>129.34244027476331</v>
       </c>
-      <c r="D4" s="9">
+      <c r="E4" s="3">
         <v>5.7981292072901276</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F4" s="3">
         <v>30.347420160428555</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G4" s="3">
         <v>44.061728168773328</v>
       </c>
-      <c r="G4" s="10">
+      <c r="H4" s="4">
         <v>145.31072184565431</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
+        <v>13988</v>
+      </c>
+      <c r="C5" s="3">
         <v>6099.5746583388254</v>
       </c>
-      <c r="C5" s="9">
+      <c r="D5" s="3">
         <v>45.5597668866777</v>
       </c>
-      <c r="D5" s="9">
+      <c r="E5" s="3">
         <v>1.454831051187979</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F5" s="3">
         <v>15.884136337524684</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="3">
         <v>24.847649636065924</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="4">
         <v>81.59798451488723</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
+        <v>18219</v>
+      </c>
+      <c r="C6" s="3">
         <v>45707.893527278051</v>
       </c>
-      <c r="C6" s="9">
+      <c r="D6" s="3">
         <v>110.24347807584493</v>
       </c>
-      <c r="D6" s="9">
+      <c r="E6" s="3">
         <v>4.4594027070110451</v>
       </c>
-      <c r="E6" s="9">
+      <c r="F6" s="3">
         <v>47.020735846237812</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="3">
         <v>55.502210065570246</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="4">
         <v>178.75911933297309</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
+        <v>15183</v>
+      </c>
+      <c r="C7" s="3">
         <v>22844.581879645437</v>
       </c>
-      <c r="C7" s="9">
+      <c r="D7" s="3">
         <v>62.163628723705827</v>
       </c>
-      <c r="D7" s="9">
+      <c r="E7" s="3">
         <v>2.624236794102929</v>
       </c>
-      <c r="E7" s="9">
+      <c r="F7" s="3">
         <v>47.188242853867571</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="3">
         <v>50.025598641241622</v>
       </c>
-      <c r="G7" s="10">
+      <c r="H7" s="4">
         <v>258.19642755752562</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8">
+        <v>35558</v>
+      </c>
+      <c r="C8" s="3">
         <v>46677.132789331365</v>
       </c>
-      <c r="C8" s="9">
+      <c r="D8" s="3">
         <v>167.4842264245261</v>
       </c>
-      <c r="D8" s="9">
+      <c r="E8" s="3">
         <v>7.7551469848900982</v>
       </c>
-      <c r="E8" s="9">
+      <c r="F8" s="3">
         <v>67.965086444803418</v>
       </c>
-      <c r="F8" s="9">
+      <c r="G8" s="3">
         <v>70.012722527525938</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="4">
         <v>287.75161544941329</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
+        <v>9412</v>
+      </c>
+      <c r="C9" s="3">
         <v>16471.314137628866</v>
       </c>
-      <c r="C9" s="9">
+      <c r="D9" s="3">
         <v>28.336503825007146</v>
       </c>
-      <c r="D9" s="9">
+      <c r="E9" s="3">
         <v>2.5601768374808076</v>
       </c>
-      <c r="E9" s="9">
+      <c r="F9" s="3">
         <v>21.810702562057706</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="3">
         <v>37.663484516513023</v>
       </c>
-      <c r="G9" s="10">
+      <c r="H9" s="4">
         <v>103.72362832766667</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10">
+        <v>17846</v>
+      </c>
+      <c r="C10" s="3">
         <v>8147.9682350091052</v>
       </c>
-      <c r="C10" s="9">
+      <c r="D10" s="3">
         <v>35.855029649450373</v>
       </c>
-      <c r="D10" s="9">
+      <c r="E10" s="3">
         <v>1.3995724853383282</v>
       </c>
-      <c r="E10" s="9">
+      <c r="F10" s="3">
         <v>21.400888183575113</v>
       </c>
-      <c r="F10" s="9">
+      <c r="G10" s="3">
         <v>36.872409436428114</v>
       </c>
-      <c r="G10" s="10">
+      <c r="H10" s="4">
         <v>125.04708834109621</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11">
+        <v>20187</v>
+      </c>
+      <c r="C11" s="3">
         <v>4868.4423457238227</v>
       </c>
-      <c r="C11" s="9">
+      <c r="D11" s="3">
         <v>101.35059180160721</v>
       </c>
-      <c r="D11" s="9">
+      <c r="E11" s="3">
         <v>5.3904573846626205</v>
       </c>
-      <c r="E11" s="9">
+      <c r="F11" s="3">
         <v>17.287399744005924</v>
       </c>
-      <c r="F11" s="9">
+      <c r="G11" s="3">
         <v>26.670319445752909</v>
       </c>
-      <c r="G11" s="10">
+      <c r="H11" s="4">
         <v>75.286339066448264</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
+        <v>18310</v>
+      </c>
+      <c r="C12" s="3">
         <v>13124.403297688712</v>
       </c>
-      <c r="C12" s="9">
+      <c r="D12" s="3">
         <v>63.232078836341586</v>
       </c>
-      <c r="D12" s="9">
+      <c r="E12" s="3">
         <v>3.2161065323383453</v>
       </c>
-      <c r="E12" s="9">
+      <c r="F12" s="3">
         <v>34.458948964924708</v>
       </c>
-      <c r="F12" s="9">
+      <c r="G12" s="3">
         <v>43.970606508992354</v>
       </c>
-      <c r="G12" s="10">
+      <c r="H12" s="4">
         <v>108.37784559001014</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
+        <v>12333</v>
+      </c>
+      <c r="C13" s="3">
         <v>50601.717389520316</v>
       </c>
-      <c r="C13" s="9">
+      <c r="D13" s="3">
         <v>666.09323625099171</v>
       </c>
-      <c r="D13" s="9">
+      <c r="E13" s="3">
         <v>2.3695604716188887</v>
       </c>
-      <c r="E13" s="9">
+      <c r="F13" s="3">
         <v>60.767914700275497</v>
       </c>
-      <c r="F13" s="9">
+      <c r="G13" s="3">
         <v>64.496606517231768</v>
       </c>
-      <c r="G13" s="10">
+      <c r="H13" s="4">
         <v>326.69898449809978</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14">
+        <v>11711</v>
+      </c>
+      <c r="C14" s="3">
         <v>17284.600112446798</v>
       </c>
-      <c r="C14" s="9">
+      <c r="D14" s="3">
         <v>29.317651426731327</v>
       </c>
-      <c r="D14" s="9">
+      <c r="E14" s="3">
         <v>1.7031509661488358</v>
       </c>
-      <c r="E14" s="9">
+      <c r="F14" s="3">
         <v>28.469408849659612</v>
       </c>
-      <c r="F14" s="9">
+      <c r="G14" s="3">
         <v>34.446991987658663</v>
       </c>
-      <c r="G14" s="10">
+      <c r="H14" s="4">
         <v>130.60363868704638</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15">
+        <v>24173</v>
+      </c>
+      <c r="C15" s="3">
         <v>5751.0714457223976</v>
       </c>
-      <c r="C15" s="9">
+      <c r="D15" s="3">
         <v>60.711048249092286</v>
       </c>
-      <c r="D15" s="9">
+      <c r="E15" s="3">
         <v>4.3128097271904817</v>
       </c>
-      <c r="E15" s="9">
+      <c r="F15" s="3">
         <v>21.059875846052904</v>
       </c>
-      <c r="F15" s="9">
+      <c r="G15" s="3">
         <v>31.479409033242739</v>
       </c>
-      <c r="G15" s="10">
+      <c r="H15" s="4">
         <v>79.358650065379507</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16">
+        <v>29826</v>
+      </c>
+      <c r="C16" s="3">
         <v>24768.490922929264</v>
       </c>
-      <c r="C16" s="9">
+      <c r="D16" s="3">
         <v>163.77776493913348</v>
       </c>
-      <c r="D16" s="9">
+      <c r="E16" s="3">
         <v>9.2135411008768511</v>
       </c>
-      <c r="E16" s="9">
+      <c r="F16" s="3">
         <v>42.749856703840585</v>
       </c>
-      <c r="F16" s="9">
+      <c r="G16" s="3">
         <v>64.684084089809005</v>
       </c>
-      <c r="G16" s="10">
+      <c r="H16" s="4">
         <v>197.11397406917325</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17">
+        <v>22892</v>
+      </c>
+      <c r="C17" s="3">
         <v>12151.194301076745</v>
       </c>
-      <c r="C17" s="9">
+      <c r="D17" s="3">
         <v>46.540697660707821</v>
       </c>
-      <c r="D17" s="9">
+      <c r="E17" s="3">
         <v>4.6770249865908262</v>
       </c>
-      <c r="E17" s="9">
+      <c r="F17" s="3">
         <v>39.659014485073129</v>
       </c>
-      <c r="F17" s="9">
+      <c r="G17" s="3">
         <v>37.748584049779495</v>
       </c>
-      <c r="G17" s="10">
+      <c r="H17" s="4">
         <v>89.642773600851854</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding data for 2021 year + modifications
</commit_message>
<xml_diff>
--- a/data/pollution_data.xlsx
+++ b/data/pollution_data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51ae962a39f43cd0/Pulpit/Marcysia/github/visualisation_geographic_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{32D97925-EDF2-4026-9521-DCAA707596EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75A1B72-4763-4CE8-B0DA-8B807BE9A658}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{32D97925-EDF2-4026-9521-DCAA707596EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A60E55A-1570-4B65-B3C7-8EC4584342B3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{464988A6-2CE5-4FD1-850F-A329DDD75F44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{464988A6-2CE5-4FD1-850F-A329DDD75F44}"/>
   </bookViews>
   <sheets>
-    <sheet name="data2020" sheetId="1" r:id="rId1"/>
-    <sheet name="data2019" sheetId="2" r:id="rId2"/>
-    <sheet name="data2018" sheetId="3" r:id="rId3"/>
-    <sheet name="data2017" sheetId="4" r:id="rId4"/>
-    <sheet name="data2016" sheetId="5" r:id="rId5"/>
+    <sheet name="data2021" sheetId="6" r:id="rId1"/>
+    <sheet name="data2020" sheetId="1" r:id="rId2"/>
+    <sheet name="data2019" sheetId="2" r:id="rId3"/>
+    <sheet name="data2018" sheetId="3" r:id="rId4"/>
+    <sheet name="data2017" sheetId="4" r:id="rId5"/>
+    <sheet name="data2016" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="24">
   <si>
     <t>kujawsko-pomorskie</t>
   </si>
@@ -107,12 +108,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="@*."/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +297,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial CE"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="18">
@@ -530,7 +537,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -700,8 +707,28 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -715,8 +742,11 @@
     <xf numFmtId="4" fontId="22" fillId="0" borderId="12" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="11" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="183">
     <cellStyle name="20% - akcent 1 2" xfId="2" xr:uid="{6E693B41-B438-4AD0-B6B6-8595771CB68F}"/>
     <cellStyle name="20% - akcent 2 2" xfId="3" xr:uid="{BCCB192B-02E7-4190-93F6-1B42E6FC4EC7}"/>
     <cellStyle name="20% - akcent 3 2" xfId="4" xr:uid="{42A7B8DC-FF87-4579-8777-CB5D2242A109}"/>
@@ -771,6 +801,7 @@
     <cellStyle name="Dziesiętny 2" xfId="37" xr:uid="{236F30FD-982C-44E7-B5DF-14BF87B865E5}"/>
     <cellStyle name="Dziesiętny 2 2" xfId="122" xr:uid="{3682C709-4755-4FD2-BDC9-4E950E177B00}"/>
     <cellStyle name="Dziesiętny 2 3" xfId="127" xr:uid="{4593CDD9-EBC6-4B1B-8ECA-78CD8A3ADC52}"/>
+    <cellStyle name="Dziesiętny 3" xfId="182" xr:uid="{5745E47F-1760-4EB9-B35A-3D376E9A5448}"/>
     <cellStyle name="Hiperłącze 2" xfId="117" xr:uid="{644E2437-A0F9-4296-9749-8CEA1AB96B8D}"/>
     <cellStyle name="Hiperłącze 2 2" xfId="121" xr:uid="{4C095A47-A019-4351-A2FA-C8851241E729}"/>
     <cellStyle name="Komórka połączona 2" xfId="39" xr:uid="{1F2A84F5-7A83-46AD-8249-F3BE44F6020F}"/>
@@ -863,22 +894,41 @@
     <cellStyle name="Walutowy 2" xfId="140" xr:uid="{2B3BD304-2B33-440A-9690-D5C4CD053916}"/>
     <cellStyle name="Walutowy 2 2" xfId="146" xr:uid="{2BD32565-8697-4E10-B709-6C7F79A6FDD0}"/>
     <cellStyle name="Walutowy 2 2 2" xfId="153" xr:uid="{0DF92D83-9883-410F-ACFC-8D8F436AAF63}"/>
+    <cellStyle name="Walutowy 2 2 2 2" xfId="174" xr:uid="{BCAFE5C5-6E82-4DF2-9D2D-B04FC34C763C}"/>
     <cellStyle name="Walutowy 2 2 3" xfId="159" xr:uid="{060F66E1-8757-4009-972F-AD9E933952B4}"/>
+    <cellStyle name="Walutowy 2 2 3 2" xfId="180" xr:uid="{DE20CD51-9BE5-4D6E-AD6B-F052AD1D3B00}"/>
+    <cellStyle name="Walutowy 2 2 4" xfId="168" xr:uid="{D0118D04-4657-49E7-B5AC-5DECC86AB632}"/>
     <cellStyle name="Walutowy 2 3" xfId="149" xr:uid="{F0B94C57-3414-473B-A43A-EAB9542BC9D3}"/>
+    <cellStyle name="Walutowy 2 3 2" xfId="170" xr:uid="{F20E0226-8158-4F9E-8400-D7AEE782077C}"/>
     <cellStyle name="Walutowy 2 4" xfId="155" xr:uid="{7ACD3F8E-0F80-4C99-8A29-47F9299D0F1A}"/>
+    <cellStyle name="Walutowy 2 4 2" xfId="176" xr:uid="{EFCC40A8-B6A7-4331-8943-1EAC4E14F6F1}"/>
+    <cellStyle name="Walutowy 2 5" xfId="164" xr:uid="{1ACA3AD1-35F7-4061-A7D8-3B32E0C01DBC}"/>
     <cellStyle name="Walutowy 3" xfId="141" xr:uid="{A72B15A8-8476-499F-906F-7D214A95DE51}"/>
     <cellStyle name="Walutowy 3 2" xfId="150" xr:uid="{60C0E57B-F368-465C-90A5-86CDC8C1AA87}"/>
+    <cellStyle name="Walutowy 3 2 2" xfId="171" xr:uid="{2710E116-E95E-4C5F-9DE5-85358C053367}"/>
     <cellStyle name="Walutowy 3 3" xfId="156" xr:uid="{FA7AC817-45F7-4705-91BF-F64383B63884}"/>
+    <cellStyle name="Walutowy 3 3 2" xfId="177" xr:uid="{3B252661-43CF-4EBB-9ABB-606BFD1B951C}"/>
+    <cellStyle name="Walutowy 3 4" xfId="165" xr:uid="{E6EFCDF7-6B1C-4BAE-B5CC-C40A796A77E6}"/>
     <cellStyle name="Walutowy 4" xfId="142" xr:uid="{326C8DD2-A2BB-4A1D-B81B-C176538637D7}"/>
     <cellStyle name="Walutowy 4 2" xfId="151" xr:uid="{57BAB5C5-EC5D-45BA-AC19-E6F698206C51}"/>
+    <cellStyle name="Walutowy 4 2 2" xfId="172" xr:uid="{628BE59B-1894-4694-ABA1-5045E4E90B1F}"/>
     <cellStyle name="Walutowy 4 3" xfId="157" xr:uid="{9B426BE3-28AB-422E-8318-1BF50A61FE75}"/>
+    <cellStyle name="Walutowy 4 3 2" xfId="178" xr:uid="{2FEA8177-6441-4986-82CF-2DD72F68BEEF}"/>
+    <cellStyle name="Walutowy 4 4" xfId="166" xr:uid="{F5CD1693-DF4D-48EB-B3BA-6AC3FB16B776}"/>
     <cellStyle name="Walutowy 5" xfId="145" xr:uid="{5A8DA708-BFCE-42B0-9CF3-5E8D6455B55C}"/>
     <cellStyle name="Walutowy 5 2" xfId="152" xr:uid="{65CEA1D1-7EEA-46D9-A175-45D845D5ECE2}"/>
+    <cellStyle name="Walutowy 5 2 2" xfId="173" xr:uid="{4039E50C-556F-4C2E-B5F9-3BA02818AF4D}"/>
     <cellStyle name="Walutowy 5 3" xfId="158" xr:uid="{E5853F02-0801-40E4-8AD7-8CE425F1984A}"/>
+    <cellStyle name="Walutowy 5 3 2" xfId="179" xr:uid="{AEFFD7E7-E492-4DCE-AB8A-621FDD7FCA19}"/>
+    <cellStyle name="Walutowy 5 4" xfId="167" xr:uid="{4099D5DD-220E-4D41-B398-0EA714B2ADFB}"/>
     <cellStyle name="Walutowy 6" xfId="148" xr:uid="{A941397B-CF72-4CDB-968B-3B351A478236}"/>
+    <cellStyle name="Walutowy 6 2" xfId="169" xr:uid="{D1439259-2224-474E-BAB0-A4483C3942A9}"/>
     <cellStyle name="Walutowy 7" xfId="154" xr:uid="{8B90669F-EDFF-4AC2-873C-F4176BC6E651}"/>
+    <cellStyle name="Walutowy 7 2" xfId="175" xr:uid="{3EDB6622-0828-4FD5-A504-04DAC06CA80E}"/>
     <cellStyle name="Walutowy 8" xfId="160" xr:uid="{80E1ECD9-E007-4DBD-A589-628B948A4344}"/>
+    <cellStyle name="Walutowy 8 2" xfId="181" xr:uid="{0ABFAD82-6B21-42D3-ABC0-43D146C893E5}"/>
     <cellStyle name="Walutowy 9" xfId="130" xr:uid="{97BBACBC-302F-4B89-B8C8-7AF7F6DE1393}"/>
+    <cellStyle name="Walutowy 9 2" xfId="163" xr:uid="{99EDAA5E-E440-4F4E-9B21-39CD2664FC94}"/>
     <cellStyle name="Złe 2" xfId="66" xr:uid="{F1783075-7586-4CB2-8EBF-E489531599FF}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1210,11 +1260,471 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768D8290-9C8E-450E-95C2-102C06C63A40}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>19947</v>
+      </c>
+      <c r="C2" s="5">
+        <v>24306.615816358069</v>
+      </c>
+      <c r="D2" s="5">
+        <v>42.204026869153992</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3.1843870391899167</v>
+      </c>
+      <c r="F2" s="5">
+        <v>26.560921439821126</v>
+      </c>
+      <c r="G2" s="5">
+        <v>37.651277054506494</v>
+      </c>
+      <c r="H2" s="5">
+        <v>158.10832251846068</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>17972</v>
+      </c>
+      <c r="C3" s="5">
+        <v>15750.880015215351</v>
+      </c>
+      <c r="D3" s="5">
+        <v>62.296392454793548</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6.1986901076185204</v>
+      </c>
+      <c r="F3" s="5">
+        <v>27.175525846029338</v>
+      </c>
+      <c r="G3" s="5">
+        <v>44.765091330559294</v>
+      </c>
+      <c r="H3" s="5">
+        <v>175.50607972904032</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>25122</v>
+      </c>
+      <c r="C4" s="5">
+        <v>12270.732091231925</v>
+      </c>
+      <c r="D4" s="5">
+        <v>130.39843603673904</v>
+      </c>
+      <c r="E4" s="5">
+        <v>6.1086024926895606</v>
+      </c>
+      <c r="F4" s="5">
+        <v>19.906974093689815</v>
+      </c>
+      <c r="G4" s="5">
+        <v>31.411580711873334</v>
+      </c>
+      <c r="H4" s="5">
+        <v>145.77615372440863</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>13988</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4986.7881240287898</v>
+      </c>
+      <c r="D5" s="5">
+        <v>40.195248621802172</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1.6823151227033093</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3.9760157499156388</v>
+      </c>
+      <c r="G5" s="5">
+        <v>12.542704591408992</v>
+      </c>
+      <c r="H5" s="5">
+        <v>61.748328446838343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>18219</v>
+      </c>
+      <c r="C6" s="5">
+        <v>48236.01115940226</v>
+      </c>
+      <c r="D6" s="5">
+        <v>93.925244986654974</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5.2649110496531968</v>
+      </c>
+      <c r="F6" s="5">
+        <v>67.253714460109336</v>
+      </c>
+      <c r="G6" s="5">
+        <v>66.620293558028294</v>
+      </c>
+      <c r="H6" s="5">
+        <v>229.62900255567612</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>15183</v>
+      </c>
+      <c r="C7" s="5">
+        <v>17924.340852277557</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45.038965273847012</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2.3539842369959358</v>
+      </c>
+      <c r="F7" s="5">
+        <v>22.781470914543895</v>
+      </c>
+      <c r="G7" s="5">
+        <v>32.441838539420907</v>
+      </c>
+      <c r="H7" s="5">
+        <v>156.95150184317555</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>35558</v>
+      </c>
+      <c r="C8" s="5">
+        <v>58045.516561057208</v>
+      </c>
+      <c r="D8" s="5">
+        <v>148.76935502356639</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9.9047243237962022</v>
+      </c>
+      <c r="F8" s="5">
+        <v>49.145645642612479</v>
+      </c>
+      <c r="G8" s="5">
+        <v>87.877852537846351</v>
+      </c>
+      <c r="H8" s="5">
+        <v>229.28154056523454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>9412</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20797.11391108618</v>
+      </c>
+      <c r="D9" s="5">
+        <v>23.123655152827151</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2.7627989547845613</v>
+      </c>
+      <c r="F9" s="5">
+        <v>13.429357855851084</v>
+      </c>
+      <c r="G9" s="5">
+        <v>25.712321672226278</v>
+      </c>
+      <c r="H9" s="5">
+        <v>68.32499066672095</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>17846</v>
+      </c>
+      <c r="C10" s="5">
+        <v>8028.3071944199346</v>
+      </c>
+      <c r="D10" s="5">
+        <v>31.420551433820236</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.5441664894682801</v>
+      </c>
+      <c r="F10" s="5">
+        <v>16.390945221629575</v>
+      </c>
+      <c r="G10" s="5">
+        <v>19.264056580944771</v>
+      </c>
+      <c r="H10" s="5">
+        <v>242.66125763273357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>20187</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4119.5083887150622</v>
+      </c>
+      <c r="D11" s="5">
+        <v>104.06876155820134</v>
+      </c>
+      <c r="E11" s="5">
+        <v>7.3177326319886751</v>
+      </c>
+      <c r="F11" s="5">
+        <v>7.1600512168196193</v>
+      </c>
+      <c r="G11" s="5">
+        <v>17.599099417891438</v>
+      </c>
+      <c r="H11" s="5">
+        <v>68.639109637131796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>18310</v>
+      </c>
+      <c r="C12" s="5">
+        <v>13564.651484275428</v>
+      </c>
+      <c r="D12" s="5">
+        <v>53.299627764049987</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3.916282586009455</v>
+      </c>
+      <c r="F12" s="5">
+        <v>23.210167712762658</v>
+      </c>
+      <c r="G12" s="5">
+        <v>35.000928201246026</v>
+      </c>
+      <c r="H12" s="5">
+        <v>161.23772516790018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>12333</v>
+      </c>
+      <c r="C13" s="5">
+        <v>50417.501395260726</v>
+      </c>
+      <c r="D13" s="5">
+        <v>488.88277149250752</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2.6095831702391781</v>
+      </c>
+      <c r="F13" s="5">
+        <v>44.30567248110507</v>
+      </c>
+      <c r="G13" s="5">
+        <v>55.835075510542396</v>
+      </c>
+      <c r="H13" s="5">
+        <v>219.66195878562249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>11711</v>
+      </c>
+      <c r="C14" s="5">
+        <v>15333.414077306219</v>
+      </c>
+      <c r="D14" s="5">
+        <v>22.974092307593676</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1.8657385508116338</v>
+      </c>
+      <c r="F14" s="5">
+        <v>16.017194439571547</v>
+      </c>
+      <c r="G14" s="5">
+        <v>22.20271235623348</v>
+      </c>
+      <c r="H14" s="5">
+        <v>68.976354709435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>24173</v>
+      </c>
+      <c r="C15" s="5">
+        <v>5524.2732389756593</v>
+      </c>
+      <c r="D15" s="5">
+        <v>58.351054657667753</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5.6651186597158603</v>
+      </c>
+      <c r="F15" s="5">
+        <v>12.094499230407983</v>
+      </c>
+      <c r="G15" s="5">
+        <v>21.25144012503549</v>
+      </c>
+      <c r="H15" s="5">
+        <v>124.79959759869078</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>29826</v>
+      </c>
+      <c r="C16" s="5">
+        <v>21070.684029961096</v>
+      </c>
+      <c r="D16" s="5">
+        <v>141.3301617718603</v>
+      </c>
+      <c r="E16" s="5">
+        <v>11.726138553544452</v>
+      </c>
+      <c r="F16" s="5">
+        <v>23.498288115069307</v>
+      </c>
+      <c r="G16" s="5">
+        <v>50.532891995858982</v>
+      </c>
+      <c r="H16" s="5">
+        <v>213.7867828532174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>22892</v>
+      </c>
+      <c r="C17" s="5">
+        <v>11199.943362083515</v>
+      </c>
+      <c r="D17" s="5">
+        <v>38.889887069766381</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.6935916550264647</v>
+      </c>
+      <c r="F17" s="5">
+        <v>19.469136843201799</v>
+      </c>
+      <c r="G17" s="5">
+        <v>30.676489368823443</v>
+      </c>
+      <c r="H17" s="5">
+        <v>195.64501570738182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7818F3A-23A1-49D0-83E8-3B6A860DDD22}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B17"/>
+      <selection activeCell="H17" sqref="A1:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1669,7 +2179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8598B8FC-B048-4239-964A-724689BBF094}">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -2129,7 +2639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4806FBA-1A1C-40A4-9BED-5BA200EFD858}">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -2589,7 +3099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2917CE5-29C7-4EC4-AAA8-6BF7913A090C}">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -3046,11 +3556,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECAE9A7-1C24-431A-8CF3-7D2D22897543}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>